<commit_message>
JSON schema for Data Type registration-- updates
</commit_message>
<xml_diff>
--- a/Definitions/Concept.xlsx
+++ b/Definitions/Concept.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Definitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\USGIN\digital-crust-LDR\Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13788"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13790"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -467,16 +467,16 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="45.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="31.88671875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="7" width="9.08984375" style="1"/>
+    <col min="8" max="8" width="31.90625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="str">
         <f>"def/concept/" &amp; LOWER(SUBSTITUTE(B2," ", "-"))</f>
         <v>def/concept/table</v>
@@ -517,7 +517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="str">
         <f t="shared" ref="A3:A11" si="0">"def/concept/" &amp; LOWER(SUBSTITUTE(B3," ", "-"))</f>
         <v>def/concept/data-object</v>
@@ -535,7 +535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/median</v>
@@ -550,7 +550,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/mean</v>
@@ -565,7 +565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/geometric-mean</v>
@@ -580,7 +580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/mode</v>
@@ -595,7 +595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/common-value</v>
@@ -613,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/primitive</v>
@@ -628,7 +628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/date-range</v>
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>def/concept/controlled-vocabulary</v>
@@ -658,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
     </row>
   </sheetData>

</xml_diff>